<commit_message>
Updated excel test data for TC-51409,40,57,59,60,61,144,145,51390
</commit_message>
<xml_diff>
--- a/Test Data/TC_144_145_Verify_Battery_Standby_And_Battery_Alarm_Limits_On_Changing_CPU_And_PSU.xlsx
+++ b/Test Data/TC_144_145_Verify_Battery_Standby_And_Battery_Alarm_Limits_On_Changing_CPU_And_PSU.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_01_02_2019\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AE81E5-8F6B-404E-A15A-1A6966B44EDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
@@ -141,7 +142,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,19 +260,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -553,7 +554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -674,11 +675,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,12 +698,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -711,17 +712,17 @@
       <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
@@ -731,13 +732,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="14"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
@@ -788,7 +789,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2">
         <v>16</v>

</xml_diff>